<commit_message>
Add GRU Model, Update Results, Add Summary for Random Forest Regressor
</commit_message>
<xml_diff>
--- a/Models/Results.xlsx
+++ b/Models/Results.xlsx
@@ -72,7 +72,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,13 +95,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -440,7 +433,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -461,6 +454,19 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -564,152 +570,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -720,15 +726,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -736,10 +736,26 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1062,7 +1078,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G5" sqref="G5:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1088,499 +1104,499 @@
     <row r="2" spans="2:11">
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="G3" s="5" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="G3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4">
         <v>0.3</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>0.2</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="4">
         <v>0.1</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4">
         <v>0.3</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="4">
         <v>0.2</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="4">
         <v>0.1</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="6">
         <v>0.8459</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <v>0.849</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="6">
         <v>0.844</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="7">
         <v>0.1897</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="7">
         <v>0.1759</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="7">
         <v>0.1782</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <v>0.9998</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <v>0.9998</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>0.9999</v>
       </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="8" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="7">
         <v>0.5835</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="7">
         <v>0.8453</v>
       </c>
-      <c r="K6" s="9">
-        <v>0.9963</v>
+      <c r="K6" s="7">
+        <v>0.9965</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>0.9514</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="7">
         <v>0.9526</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <v>0.9505</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="7">
         <v>0.0248</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="7">
         <v>0.0315</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="7">
         <v>0.0412</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8" t="s">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>0.9999</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="7">
         <v>0.9999</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>0.9999</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="8" t="s">
+      <c r="G12" s="5"/>
+      <c r="H12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="7">
         <v>0.999</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="7">
         <v>0.9991</v>
       </c>
-      <c r="K12" s="9">
-        <v>0.9991</v>
+      <c r="K12" s="7">
+        <v>0.9953</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="7">
         <v>0.7674</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="7">
         <v>0.77</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="7">
         <v>0.7695</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="8" t="s">
+      <c r="H17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="7">
         <v>0.1835</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="7">
         <v>0.202</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="7">
         <v>0.2083</v>
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8" t="s">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="7">
         <v>0.9998</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="7">
         <v>0.9998</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="7">
         <v>0.9998</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="8" t="s">
+      <c r="G18" s="5"/>
+      <c r="H18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="14">
         <v>0.9966</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="7">
         <v>0.9975</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="7">
         <v>0.9979</v>
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="7">
         <v>0.3451</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="7">
         <v>0.3363</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="7">
         <v>0.322</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="H23" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I23" s="9">
+      <c r="I23" s="15">
         <v>0.0267</v>
       </c>
-      <c r="J23" s="9">
+      <c r="J23" s="15">
         <v>0.0278</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K23" s="15">
         <v>0.0305</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="10"/>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="7">
         <v>0.9962</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="7">
         <v>0.998</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="7">
         <v>0.9965</v>
       </c>
-      <c r="G24" s="10"/>
-      <c r="H24" s="8" t="s">
+      <c r="G24" s="11"/>
+      <c r="H24" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="15">
         <v>0.9946</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="15">
         <v>0.9942</v>
       </c>
-      <c r="K24" s="9">
-        <v>0.9927</v>
+      <c r="K24" s="15">
+        <v>0.9952</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="10"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="10"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="10"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="10"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
     </row>
     <row r="29" spans="7:11">
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>

<commit_message>
Update GRU model and results
</commit_message>
<xml_diff>
--- a/Models/Results.xlsx
+++ b/Models/Results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
   <si>
     <t>CPU Usage</t>
   </si>
@@ -53,6 +53,9 @@
     <t>Random Forest Regressor</t>
   </si>
   <si>
+    <t>GRU</t>
+  </si>
+  <si>
     <t>Echo Service</t>
   </si>
   <si>
@@ -72,7 +75,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,17 +84,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -433,7 +441,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -454,19 +462,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -585,177 +580,193 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1078,7 +1089,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G10"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1166,13 +1177,13 @@
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
         <v>0.8459</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <v>0.849</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="7">
         <v>0.844</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -1181,422 +1192,486 @@
       <c r="H5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="9">
         <v>0.1897</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="9">
         <v>0.1759</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="9">
         <v>0.1782</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="5"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="9">
         <v>0.9998</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="9">
         <v>0.9998</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="9">
         <v>0.9999</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="9">
         <v>0.5835</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="9">
         <v>0.8453</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="9">
         <v>0.9965</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.9987</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.9978</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0.9938</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0.4664</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0.4053</v>
+      </c>
+      <c r="K7" s="10">
+        <v>0.3039</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="9">
         <v>0.9514</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="9">
         <v>0.9526</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="9">
         <v>0.9505</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="9">
         <v>0.0248</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="9">
         <v>0.0315</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="9">
         <v>0.0412</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="5"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="9">
         <v>0.9999</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="9">
         <v>0.9999</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="9">
         <v>0.9999</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="8"/>
       <c r="H12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="9">
         <v>0.999</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="9">
         <v>0.9991</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="9">
         <v>0.9953</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="11">
+        <v>0.9993</v>
+      </c>
+      <c r="D13" s="11">
+        <v>0.9992</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0.9973</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0.5156</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0.4883</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0.4335</v>
+      </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="6"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="9">
         <v>0.7674</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="9">
         <v>0.77</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="9">
         <v>0.7695</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="9">
         <v>0.1835</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="9">
         <v>0.202</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="9">
         <v>0.2083</v>
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="5"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="9">
         <v>0.9998</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="9">
         <v>0.9998</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="9">
         <v>0.9998</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="8"/>
       <c r="H18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="14">
+      <c r="I18" s="20">
         <v>0.9966</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="9">
         <v>0.9975</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="9">
         <v>0.9979</v>
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0.9979</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0.9989</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.9974</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="10">
+        <v>0.6078</v>
+      </c>
+      <c r="J19" s="10">
+        <v>0.5939</v>
+      </c>
+      <c r="K19" s="10">
+        <v>0.4859</v>
+      </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-      <c r="K21" s="6"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
       <c r="G22" s="8"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="10" t="s">
-        <v>10</v>
+      <c r="A23" s="13" t="s">
+        <v>11</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="9">
         <v>0.3451</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="9">
         <v>0.3363</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="9">
         <v>0.322</v>
       </c>
-      <c r="G23" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="12" t="s">
+      <c r="G23" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="I23" s="15">
+      <c r="I23" s="21">
         <v>0.0267</v>
       </c>
-      <c r="J23" s="15">
+      <c r="J23" s="21">
         <v>0.0278</v>
       </c>
-      <c r="K23" s="15">
+      <c r="K23" s="21">
         <v>0.0305</v>
       </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="10"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="9">
         <v>0.9962</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="9">
         <v>0.998</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="9">
         <v>0.9965</v>
       </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="12" t="s">
+      <c r="G24" s="17"/>
+      <c r="H24" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="15">
+      <c r="I24" s="21">
         <v>0.9946</v>
       </c>
-      <c r="J24" s="15">
+      <c r="J24" s="21">
         <v>0.9942</v>
       </c>
-      <c r="K24" s="15">
+      <c r="K24" s="21">
         <v>0.9952</v>
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="10"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0.9712</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0.9738</v>
+      </c>
+      <c r="E25" s="10">
+        <v>0.9692</v>
+      </c>
+      <c r="G25" s="17"/>
+      <c r="H25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="10">
+        <v>0.9921</v>
+      </c>
+      <c r="J25" s="10">
+        <v>0.9924</v>
+      </c>
+      <c r="K25" s="10">
+        <v>0.985</v>
+      </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="10"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="10"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="10"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
     </row>
     <row r="29" spans="7:11">
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>

<commit_message>
Update Random Forest Regressor Results
</commit_message>
<xml_diff>
--- a/Models/Results.xlsx
+++ b/Models/Results.xlsx
@@ -710,7 +710,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -729,12 +729,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -742,9 +736,6 @@
       <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -753,19 +744,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1089,7 +1070,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1177,13 +1158,13 @@
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>0.8459</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>0.849</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>0.844</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -1192,107 +1173,107 @@
       <c r="H5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="7">
         <v>0.1897</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="7">
         <v>0.1759</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="7">
         <v>0.1782</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="8"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <v>0.9998</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="7">
         <v>0.9998</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>0.9999</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="7">
         <v>0.5835</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="7">
         <v>0.8453</v>
       </c>
-      <c r="K6" s="9">
-        <v>0.9965</v>
+      <c r="K6" s="7">
+        <v>0.7503</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="8"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="8">
         <v>0.9987</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="8">
         <v>0.9978</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="8">
         <v>0.9938</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="8">
         <v>0.4664</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J7" s="8">
         <v>0.4053</v>
       </c>
-      <c r="K7" s="10">
+      <c r="K7" s="8">
         <v>0.3039</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="8"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="8"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="8"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="5" t="s">
@@ -1301,13 +1282,13 @@
       <c r="B11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>0.9514</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="7">
         <v>0.9526</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <v>0.9505</v>
       </c>
       <c r="G11" s="5" t="s">
@@ -1316,107 +1297,107 @@
       <c r="H11" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="7">
         <v>0.0248</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="7">
         <v>0.0315</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="7">
         <v>0.0412</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="8"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>0.9999</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="7">
         <v>0.9999</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>0.9999</v>
       </c>
-      <c r="G12" s="8"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="7">
         <v>0.999</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="7">
         <v>0.9991</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="7">
         <v>0.9953</v>
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="8"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="11">
+      <c r="C13" s="9">
         <v>0.9993</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="9">
         <v>0.9992</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="9">
         <v>0.9973</v>
       </c>
-      <c r="G13" s="8"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="10">
+      <c r="I13" s="8">
         <v>0.5156</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="8">
         <v>0.4883</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="8">
         <v>0.4335</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="8"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="8"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="8"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="5" t="s">
@@ -1425,13 +1406,13 @@
       <c r="B17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="7">
         <v>0.7674</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="7">
         <v>0.77</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="7">
         <v>0.7695</v>
       </c>
       <c r="G17" s="5" t="s">
@@ -1440,238 +1421,238 @@
       <c r="H17" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="7">
         <v>0.1835</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="7">
         <v>0.202</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="7">
         <v>0.2083</v>
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="8"/>
+      <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="7">
         <v>0.9998</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D18" s="7">
         <v>0.9998</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="7">
         <v>0.9998</v>
       </c>
-      <c r="G18" s="8"/>
+      <c r="G18" s="5"/>
       <c r="H18" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I18" s="20">
+      <c r="I18" s="8">
         <v>0.9966</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="7">
         <v>0.9975</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="7">
         <v>0.9979</v>
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="8"/>
+      <c r="A19" s="5"/>
       <c r="B19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="8">
         <v>0.9979</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="8">
         <v>0.9989</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="8">
         <v>0.9974</v>
       </c>
-      <c r="G19" s="8"/>
+      <c r="G19" s="5"/>
       <c r="H19" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="8">
         <v>0.6078</v>
       </c>
-      <c r="J19" s="10">
+      <c r="J19" s="8">
         <v>0.5939</v>
       </c>
-      <c r="K19" s="10">
+      <c r="K19" s="8">
         <v>0.4859</v>
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="8"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="8"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="8"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="7">
         <v>0.3451</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23" s="7">
         <v>0.3363</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="7">
         <v>0.322</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="15" t="s">
+      <c r="H23" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I23" s="21">
+      <c r="I23" s="14">
         <v>0.0267</v>
       </c>
-      <c r="J23" s="21">
+      <c r="J23" s="14">
         <v>0.0278</v>
       </c>
-      <c r="K23" s="21">
+      <c r="K23" s="14">
         <v>0.0305</v>
       </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="16"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="7">
         <v>0.9962</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="7">
         <v>0.998</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="7">
         <v>0.9965</v>
       </c>
-      <c r="G24" s="17"/>
-      <c r="H24" s="15" t="s">
+      <c r="G24" s="11"/>
+      <c r="H24" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I24" s="21">
+      <c r="I24" s="14">
         <v>0.9946</v>
       </c>
-      <c r="J24" s="21">
+      <c r="J24" s="14">
         <v>0.9942</v>
       </c>
-      <c r="K24" s="21">
-        <v>0.9952</v>
+      <c r="K24" s="14">
+        <v>0.9907</v>
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="16"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="8">
         <v>0.9712</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="8">
         <v>0.9738</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E25" s="8">
         <v>0.9692</v>
       </c>
-      <c r="G25" s="17"/>
+      <c r="G25" s="11"/>
       <c r="H25" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I25" s="10">
+      <c r="I25" s="8">
         <v>0.9921</v>
       </c>
-      <c r="J25" s="10">
+      <c r="J25" s="8">
         <v>0.9924</v>
       </c>
-      <c r="K25" s="10">
+      <c r="K25" s="8">
         <v>0.985</v>
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="16"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="16"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="16"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
     </row>
     <row r="29" spans="7:11">
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>

<commit_message>
Update results and XGBoost Model
</commit_message>
<xml_diff>
--- a/Models/Results.xlsx
+++ b/Models/Results.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="13">
   <si>
     <t>CPU Usage</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>GRU</t>
+  </si>
+  <si>
+    <t>LightGBM</t>
   </si>
   <si>
     <t>Echo Service</t>
@@ -1070,7 +1073,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1241,15 +1244,31 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="B8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.9677</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.8472</v>
+      </c>
+      <c r="E8" s="6">
+        <v>-0.1209</v>
+      </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="H8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0.3265</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0.4122</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0.3068</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" s="5"/>
@@ -1277,7 +1296,7 @@
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>6</v>
@@ -1292,7 +1311,7 @@
         <v>0.9505</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>6</v>
@@ -1365,15 +1384,31 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.9988</v>
+      </c>
+      <c r="D14" s="6">
+        <v>0.9972</v>
+      </c>
+      <c r="E14" s="6">
+        <v>0.9885</v>
+      </c>
       <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
+      <c r="H14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I14" s="6">
+        <v>0.4671</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0.4466</v>
+      </c>
+      <c r="K14" s="6">
+        <v>0.3547</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="5"/>
@@ -1401,7 +1436,7 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>6</v>
@@ -1416,7 +1451,7 @@
         <v>0.7695</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>6</v>
@@ -1489,15 +1524,31 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="B20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.9871</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.9956</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.9839</v>
+      </c>
       <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
+      <c r="H20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.5615</v>
+      </c>
+      <c r="J20" s="6">
+        <v>0.5649</v>
+      </c>
+      <c r="K20" s="6">
+        <v>0.4557</v>
+      </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="5"/>
@@ -1525,7 +1576,7 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>6</v>
@@ -1540,7 +1591,7 @@
         <v>0.322</v>
       </c>
       <c r="G23" s="11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>6</v>
@@ -1613,15 +1664,31 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="10"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="B26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="6">
+        <v>0.9571</v>
+      </c>
+      <c r="D26" s="6">
+        <v>0.9729</v>
+      </c>
+      <c r="E26" s="6">
+        <v>0.961</v>
+      </c>
       <c r="G26" s="11"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
+      <c r="H26" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="12">
+        <v>0.8687</v>
+      </c>
+      <c r="J26" s="12">
+        <v>0.8094</v>
+      </c>
+      <c r="K26" s="12">
+        <v>0.9785</v>
+      </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="10"/>

</xml_diff>